<commit_message>
Started processing new dataset
</commit_message>
<xml_diff>
--- a/Python/Assessment.xlsx
+++ b/Python/Assessment.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanorgan/Desktop/BU/Classes/Combined Final/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31476398-2572-1943-9BFC-14ACED265EFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD95A8C-B7F1-3F4F-AC92-B5F5599DB568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="860" windowWidth="27640" windowHeight="15560" xr2:uid="{9CCA3859-451F-2F48-8D09-505DC1F3A4A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -531,7 +531,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Making scripts to generatee some graphics
</commit_message>
<xml_diff>
--- a/Python/Assessment.xlsx
+++ b/Python/Assessment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanorgan/Desktop/BU/Classes/Combined Final/Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD95A8C-B7F1-3F4F-AC92-B5F5599DB568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C373BCBD-6662-5D4C-94A0-EE95BD56B893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="860" windowWidth="27640" windowHeight="15560" xr2:uid="{9CCA3859-451F-2F48-8D09-505DC1F3A4A8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="64">
   <si>
     <t>Person</t>
   </si>
@@ -177,6 +177,57 @@
   </si>
   <si>
     <t>Hans Zimmer</t>
+  </si>
+  <si>
+    <t>Classifier</t>
+  </si>
+  <si>
+    <t>Music Data</t>
+  </si>
+  <si>
+    <t>Playlist</t>
+  </si>
+  <si>
+    <t>Refined Playlist</t>
+  </si>
+  <si>
+    <t>Dreams</t>
+  </si>
+  <si>
+    <t>'The Rippingtons', 'Russ Freeman', 'David Benoit', 'David Koz', 'Gregg Karukas', 'Jimmy Johnson', 'Tony Morales', 'Steve Reid'</t>
+  </si>
+  <si>
+    <t>Radioactive</t>
+  </si>
+  <si>
+    <t>Imagine Dragons</t>
+  </si>
+  <si>
+    <t>Ho Hey</t>
+  </si>
+  <si>
+    <t>Lumineers</t>
+  </si>
+  <si>
+    <t>Daft Punk</t>
+  </si>
+  <si>
+    <t>Harder, Better, Faster, Stronger</t>
+  </si>
+  <si>
+    <t>Istanbul (Not Constantinople)</t>
+  </si>
+  <si>
+    <t>The Four Lads</t>
+  </si>
+  <si>
+    <t>Voyager</t>
+  </si>
+  <si>
+    <t>Royals</t>
+  </si>
+  <si>
+    <t>Lorde</t>
   </si>
 </sst>
 </file>
@@ -192,12 +243,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -212,8 +275,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,278 +593,570 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63AC023-F74F-1243-AFF2-E4EC120D062D}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="7.33203125" customWidth="1"/>
-    <col min="4" max="4" width="34.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31" customWidth="1"/>
-    <col min="6" max="6" width="39.33203125" customWidth="1"/>
-    <col min="7" max="7" width="24.5" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" customWidth="1"/>
+    <col min="3" max="4" width="7.33203125" customWidth="1"/>
+    <col min="5" max="5" width="34.33203125" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="7" max="7" width="39.33203125" customWidth="1"/>
+    <col min="8" max="8" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
         <v>17924</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>30753</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
         <v>50106</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>20</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
         <v>9625</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>23</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>24</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>25</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6">
         <v>106893</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>37</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>38</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7">
         <v>106889</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>29</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>39</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>40</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8">
         <v>112232</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>32</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>41</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>42</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9">
         <v>19515</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>33</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>34</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>43</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>44</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10">
         <v>19520</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>36</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>45</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>46</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>30753</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>30753</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="2">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>30753</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>15851</v>
+      </c>
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>15851</v>
+      </c>
+      <c r="E15" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>15851</v>
+      </c>
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" t="s">
+        <v>61</v>
+      </c>
+      <c r="H16" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>9625</v>
+      </c>
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H17" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>9625</v>
+      </c>
+      <c r="E18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>9625</v>
+      </c>
+      <c r="E19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" t="s">
+        <v>62</v>
+      </c>
+      <c r="H19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>